<commit_message>
VRT Project Updated with UM1 issue fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/UserManagementTestData.xlsx
+++ b/src/test/resources/TestData/UserManagementTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC68B818-0443-4F5D-AE40-61AE2DCA822C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEC744B-B72F-4315-B48C-59448CAB374D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="900" firstSheet="1" activeTab="11" xr2:uid="{FFF56094-AA49-43C9-8779-4520FC744D16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="900" firstSheet="3" activeTab="12" xr2:uid="{FFF56094-AA49-43C9-8779-4520FC744D16}"/>
   </bookViews>
   <sheets>
     <sheet name="tcADMN008" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <sheet name="tcADMN026" sheetId="14" r:id="rId9"/>
     <sheet name="tcADMN028" sheetId="17" r:id="rId10"/>
     <sheet name="tcADMN029" sheetId="18" r:id="rId11"/>
-    <sheet name="maxuser" sheetId="19" r:id="rId12"/>
+    <sheet name="tcADMN037F" sheetId="20" r:id="rId12"/>
+    <sheet name="tcADMN067A" sheetId="21" r:id="rId13"/>
+    <sheet name="maxuser" sheetId="19" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3693" uniqueCount="1051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3713" uniqueCount="1063">
   <si>
     <t>Name</t>
   </si>
@@ -3189,6 +3191,42 @@
   </si>
   <si>
     <t>500</t>
+  </si>
+  <si>
+    <t>AName</t>
+  </si>
+  <si>
+    <t>AID</t>
+  </si>
+  <si>
+    <t>AType</t>
+  </si>
+  <si>
+    <t>Amanufacturer</t>
+  </si>
+  <si>
+    <t>ALocation</t>
+  </si>
+  <si>
+    <t>ADMIN037F</t>
+  </si>
+  <si>
+    <t>037F</t>
+  </si>
+  <si>
+    <t>HeatBath</t>
+  </si>
+  <si>
+    <t>HTC</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>ADMIN067A</t>
+  </si>
+  <si>
+    <t>067A</t>
   </si>
 </sst>
 </file>
@@ -3298,7 +3336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3371,6 +3409,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3922,10 +3963,111 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E04850E-B624-4F0F-BC78-6F4F2DD42CE5}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B727272E-AEA2-454D-A669-B18F4FD5D59F}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D02E641-C7ED-4240-9174-2722394A9E3F}">
   <dimension ref="A1:H500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
VRT Project updated with UM2 class updated with ADMN062 TC issue fixed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/UserManagementTestData.xlsx
+++ b/src/test/resources/TestData/UserManagementTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEC744B-B72F-4315-B48C-59448CAB374D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4769904B-0803-43D2-9FC1-B38F9CB16D66}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="900" firstSheet="3" activeTab="12" xr2:uid="{FFF56094-AA49-43C9-8779-4520FC744D16}"/>
   </bookViews>
@@ -25,8 +25,9 @@
     <sheet name="tcADMN028" sheetId="17" r:id="rId10"/>
     <sheet name="tcADMN029" sheetId="18" r:id="rId11"/>
     <sheet name="tcADMN037F" sheetId="20" r:id="rId12"/>
-    <sheet name="tcADMN067A" sheetId="21" r:id="rId13"/>
-    <sheet name="maxuser" sheetId="19" r:id="rId14"/>
+    <sheet name="tcADMN062" sheetId="22" r:id="rId13"/>
+    <sheet name="tcADMN067A" sheetId="21" r:id="rId14"/>
+    <sheet name="maxuser" sheetId="19" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3713" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3723" uniqueCount="1065">
   <si>
     <t>Name</t>
   </si>
@@ -3227,6 +3228,12 @@
   </si>
   <si>
     <t>067A</t>
+  </si>
+  <si>
+    <t>ADMIN062</t>
+  </si>
+  <si>
+    <t>062</t>
   </si>
 </sst>
 </file>
@@ -4015,10 +4022,59 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F9B2026-14CD-4EAC-BA6F-5B631C702D2B}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B727272E-AEA2-454D-A669-B18F4FD5D59F}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4063,7 +4119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D02E641-C7ED-4240-9174-2722394A9E3F}">
   <dimension ref="A1:H500"/>
   <sheetViews>

</xml_diff>

<commit_message>
VRT Project Updated with UM1/2/3 issues fixed and commiting to the local branch repo
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/UserManagementTestData.xlsx
+++ b/src/test/resources/TestData/UserManagementTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSC\git\VRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4769904B-0803-43D2-9FC1-B38F9CB16D66}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650068AE-A31C-429E-83A5-51810626C00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="900" firstSheet="3" activeTab="12" xr2:uid="{FFF56094-AA49-43C9-8779-4520FC744D16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="900" firstSheet="7" activeTab="16" xr2:uid="{FFF56094-AA49-43C9-8779-4520FC744D16}"/>
   </bookViews>
   <sheets>
     <sheet name="tcADMN008" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,10 @@
     <sheet name="tcADMN037F" sheetId="20" r:id="rId12"/>
     <sheet name="tcADMN062" sheetId="22" r:id="rId13"/>
     <sheet name="tcADMN067A" sheetId="21" r:id="rId14"/>
-    <sheet name="maxuser" sheetId="19" r:id="rId15"/>
+    <sheet name="tcADMN069F" sheetId="24" r:id="rId15"/>
+    <sheet name="tcADMN069G" sheetId="25" r:id="rId16"/>
+    <sheet name="tcADMN074" sheetId="26" r:id="rId17"/>
+    <sheet name="maxuser" sheetId="19" r:id="rId18"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3723" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3753" uniqueCount="1071">
   <si>
     <t>Name</t>
   </si>
@@ -3218,9 +3221,6 @@
     <t>HeatBath</t>
   </si>
   <si>
-    <t>HTC</t>
-  </si>
-  <si>
     <t>Hyderabad</t>
   </si>
   <si>
@@ -3234,6 +3234,27 @@
   </si>
   <si>
     <t>062</t>
+  </si>
+  <si>
+    <t>Htc</t>
+  </si>
+  <si>
+    <t>ADMIN069F</t>
+  </si>
+  <si>
+    <t>069F</t>
+  </si>
+  <si>
+    <t>ADMIN069G</t>
+  </si>
+  <si>
+    <t>069G</t>
+  </si>
+  <si>
+    <t>ADMIN074</t>
+  </si>
+  <si>
+    <t>074</t>
   </si>
 </sst>
 </file>
@@ -3974,7 +3995,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,10 +4031,10 @@
         <v>1058</v>
       </c>
       <c r="D2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>1059</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>1060</v>
       </c>
     </row>
   </sheetData>
@@ -4025,8 +4046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F9B2026-14CD-4EAC-BA6F-5B631C702D2B}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4050,19 +4071,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>1063</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>1064</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>1058</v>
       </c>
       <c r="D2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>1059</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>1060</v>
       </c>
     </row>
   </sheetData>
@@ -4075,7 +4096,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4099,19 +4120,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>1061</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>1062</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>1058</v>
       </c>
       <c r="D2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>1059</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>1060</v>
       </c>
     </row>
   </sheetData>
@@ -4120,6 +4141,162 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A615B69D-ECD7-479F-A638-0A0BDE77938E}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D276E4D-CCB5-4781-B05D-EEBEAEF86FFB}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E321FFF1-5D86-489F-B910-4B4DF0D0B486}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D02E641-C7ED-4240-9174-2722394A9E3F}">
   <dimension ref="A1:H500"/>
   <sheetViews>

</xml_diff>

<commit_message>
VRT Project updated with lot of changes with respect to execution in VRT build 1.1.0.7.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/UserManagementTestData.xlsx
+++ b/src/test/resources/TestData/UserManagementTestData.xlsx
@@ -8,29 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSC\git\VRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650068AE-A31C-429E-83A5-51810626C00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714D5FC6-1C5B-4B8A-9B14-BBE80146E7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="900" firstSheet="7" activeTab="16" xr2:uid="{FFF56094-AA49-43C9-8779-4520FC744D16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="900" xr2:uid="{FFF56094-AA49-43C9-8779-4520FC744D16}"/>
   </bookViews>
   <sheets>
-    <sheet name="tcADMN008" sheetId="1" r:id="rId1"/>
-    <sheet name="tcADMN009" sheetId="2" r:id="rId2"/>
-    <sheet name="tcADMN010" sheetId="3" r:id="rId3"/>
-    <sheet name="tcADMN011" sheetId="4" r:id="rId4"/>
-    <sheet name="tcADMN012" sheetId="5" r:id="rId5"/>
-    <sheet name="tcADMN021" sheetId="8" r:id="rId6"/>
-    <sheet name="tcADMN022" sheetId="9" r:id="rId7"/>
-    <sheet name="tcADMN025" sheetId="13" r:id="rId8"/>
-    <sheet name="tcADMN026" sheetId="14" r:id="rId9"/>
-    <sheet name="tcADMN028" sheetId="17" r:id="rId10"/>
-    <sheet name="tcADMN029" sheetId="18" r:id="rId11"/>
-    <sheet name="tcADMN037F" sheetId="20" r:id="rId12"/>
-    <sheet name="tcADMN062" sheetId="22" r:id="rId13"/>
-    <sheet name="tcADMN067A" sheetId="21" r:id="rId14"/>
-    <sheet name="tcADMN069F" sheetId="24" r:id="rId15"/>
-    <sheet name="tcADMN069G" sheetId="25" r:id="rId16"/>
-    <sheet name="tcADMN074" sheetId="26" r:id="rId17"/>
-    <sheet name="maxuser" sheetId="19" r:id="rId18"/>
+    <sheet name="LOGIN_024" sheetId="27" r:id="rId1"/>
+    <sheet name="tcADMN008" sheetId="1" r:id="rId2"/>
+    <sheet name="tcADMN009" sheetId="2" r:id="rId3"/>
+    <sheet name="tcADMN010" sheetId="3" r:id="rId4"/>
+    <sheet name="tcADMN011" sheetId="4" r:id="rId5"/>
+    <sheet name="tcADMN012" sheetId="5" r:id="rId6"/>
+    <sheet name="tcADMN021" sheetId="8" r:id="rId7"/>
+    <sheet name="tcADMN022" sheetId="9" r:id="rId8"/>
+    <sheet name="tcADMN025" sheetId="13" r:id="rId9"/>
+    <sheet name="tcADMN026" sheetId="14" r:id="rId10"/>
+    <sheet name="tcADMN028" sheetId="17" r:id="rId11"/>
+    <sheet name="tcADMN029" sheetId="18" r:id="rId12"/>
+    <sheet name="tcADMN037F" sheetId="20" r:id="rId13"/>
+    <sheet name="tcADMN062" sheetId="22" r:id="rId14"/>
+    <sheet name="tcADMN067A" sheetId="21" r:id="rId15"/>
+    <sheet name="tcADMN069F" sheetId="24" r:id="rId16"/>
+    <sheet name="tcADMN069G" sheetId="25" r:id="rId17"/>
+    <sheet name="tcADMN074" sheetId="26" r:id="rId18"/>
+    <sheet name="maxuser" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3753" uniqueCount="1071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3768" uniqueCount="1071">
   <si>
     <t>Name</t>
   </si>
@@ -3292,7 +3293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3335,6 +3336,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3364,7 +3371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3440,6 +3447,9 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3754,78 +3764,168 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6844256-8549-4F29-AEC2-F3718E7B5845}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85318551-19C4-4651-86D5-A01FCD0BEDC6}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="63.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>62</v>
+      </c>
+      <c r="C2" s="8">
+        <v>111111</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>449</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>449</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{C2121726-AE2A-4D97-882A-5FB9B5AADAC6}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{AFFCC87A-E49C-4FD7-8083-6DCC84B70D52}"/>
-  </hyperlinks>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300FA0F9-C58F-4C27-AA27-2C4C705A017F}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{EA57F7E5-887A-4AEA-A8DA-CC820CE0A393}"/>
+    <hyperlink ref="C2:D2" r:id="rId2" display="Welcome5@AM" xr:uid="{D92C17F5-900E-40DC-AA43-338D8390D3CE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497D9F06-C61B-42E6-9F7B-8B3F90BB191B}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -3911,7 +4011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F292CD-DD2E-4F85-9B62-1ECD3B744AB0}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -3990,7 +4090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E04850E-B624-4F0F-BC78-6F4F2DD42CE5}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4042,7 +4142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F9B2026-14CD-4EAC-BA6F-5B631C702D2B}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4091,7 +4191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B727272E-AEA2-454D-A669-B18F4FD5D59F}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4140,7 +4240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A615B69D-ECD7-479F-A638-0A0BDE77938E}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4192,7 +4292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D276E4D-CCB5-4781-B05D-EEBEAEF86FFB}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4244,11 +4344,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E321FFF1-5D86-489F-B910-4B4DF0D0B486}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4296,7 +4396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D02E641-C7ED-4240-9174-2722394A9E3F}">
   <dimension ref="A1:H500"/>
   <sheetViews>
@@ -17320,6 +17420,78 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6844256-8549-4F29-AEC2-F3718E7B5845}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{C2121726-AE2A-4D97-882A-5FB9B5AADAC6}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{AFFCC87A-E49C-4FD7-8083-6DCC84B70D52}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454D3435-3578-43C7-9257-8386301BE45D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -17384,7 +17556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D45820-850F-4509-AC94-52EF65FB8800}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -17574,7 +17746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828ED7CA-A5E7-42AA-9988-3D2A4554DADC}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -17638,7 +17810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085DC14B-8E32-4F79-8AE0-D17B1FBB9EC7}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -17711,7 +17883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC3C7EE-407E-4327-AA5D-6BA458EBDC28}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -17776,7 +17948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276B0B36-A61C-445F-BE6E-42C476FED9AF}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -17847,7 +18019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B5335B6-CB8D-48D6-B8DE-668C59B57752}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -17925,90 +18097,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300FA0F9-C58F-4C27-AA27-2C4C705A017F}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="27.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{EA57F7E5-887A-4AEA-A8DA-CC820CE0A393}"/>
-    <hyperlink ref="C2:D2" r:id="rId2" display="Welcome5@AM" xr:uid="{D92C17F5-900E-40DC-AA43-338D8390D3CE}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>